<commit_message>
10 swex unit list (#23)
* changing unit_master_id to com2us_id

* spd buff changed to .33

* change spd buff to .33

* synergies reports

adding synergies reports
adjusted unit_combat_speeds and s_other for buffs, debuffs
</commit_message>
<xml_diff>
--- a/summoners_war_0_1_0/input/settings/s_other.xlsx
+++ b/summoners_war_0_1_0/input/settings/s_other.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="7800" windowHeight="3870"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="7800" windowHeight="3870"/>
   </bookViews>
   <sheets>
     <sheet name="s_player_unit" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,14 @@
   </sheets>
   <definedNames>
     <definedName name="content_select">OFFSET(s_content!$F$2,,,COUNTIF(s_content!$F$2:$F$2000,"?*"))</definedName>
-    <definedName name="players_units_select">OFFSET(s_player_unit!$AU$2,,,COUNTIF(s_player_unit!$AU$2:$AU$2000,"?*"))</definedName>
+    <definedName name="players_units_select">OFFSET(s_player_unit!#REF!,,,COUNTIF(s_player_unit!#REF!,"?*"))</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>unit_id</t>
   </si>
@@ -137,12 +137,18 @@
     <t>spd_tune_buffer</t>
   </si>
   <si>
+    <t>buffs</t>
+  </si>
+  <si>
     <t>spd_tune_strip</t>
   </si>
   <si>
     <t>spd_tune_debuff</t>
   </si>
   <si>
+    <t>debuffs</t>
+  </si>
+  <si>
     <t>spd_tune_dmg</t>
   </si>
   <si>
@@ -152,9 +158,6 @@
     <t>reviver</t>
   </si>
   <si>
-    <t>controller</t>
-  </si>
-  <si>
     <t>runed_as_healer</t>
   </si>
   <si>
@@ -167,9 +170,6 @@
     <t>player_unit_select_ignore</t>
   </si>
   <si>
-    <t>Astar (Fire Magic Knight)</t>
-  </si>
-  <si>
     <t>content_id</t>
   </si>
   <si>
@@ -393,16 +393,13 @@
   </si>
   <si>
     <t>World Arena, Real-Time Arena</t>
-  </si>
-  <si>
-    <t>Astar (Fire Magic Knight) lvl 40 | 99999</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,8 +415,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,11 +437,35 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -445,19 +474,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -501,6 +536,16 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <strike val="0"/>
@@ -510,10 +555,17 @@
         <shadow val="0"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -529,59 +581,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="t_players_units" displayName="t_players_units" ref="A1:AU1048073" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="A1:AU1048073"/>
-  <sortState ref="A2:D150">
-    <sortCondition ref="B1:B1048576"/>
-  </sortState>
-  <tableColumns count="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AV1048414" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+  <autoFilter ref="A1:AV1048414"/>
+  <tableColumns count="48">
     <tableColumn id="1" name="unit_id"/>
-    <tableColumn id="3" name="name_ignore"/>
-    <tableColumn id="2" name="lvl_ignore"/>
-    <tableColumn id="25" name="use_for_gb12"/>
-    <tableColumn id="24" name="use_for_db12"/>
-    <tableColumn id="17" name="use_for_nb12"/>
-    <tableColumn id="16" name="use_for_sf10"/>
-    <tableColumn id="14" name="use_for_pc10"/>
-    <tableColumn id="11" name="use_for_toa"/>
-    <tableColumn id="31" name="use_for_dhole_griffon"/>
-    <tableColumn id="30" name="use_for_dhole_inugami"/>
-    <tableColumn id="29" name="use_for_dhole_warbear"/>
-    <tableColumn id="28" name="use_for_dhole_fairy"/>
-    <tableColumn id="27" name="use_for_dhole_pixie"/>
-    <tableColumn id="26" name="use_for_dhole_werewolf"/>
-    <tableColumn id="36" name="use_for_dhole_cat"/>
-    <tableColumn id="35" name="use_for_dhole_howl"/>
-    <tableColumn id="34" name="use_for_dhole_grim"/>
-    <tableColumn id="33" name="use_for_dhole_karzhan"/>
-    <tableColumn id="32" name="use_for_dhole_ellunia"/>
-    <tableColumn id="38" name="use_for_dhole_lumel"/>
-    <tableColumn id="37" name="use_for_dhole_khalderun"/>
-    <tableColumn id="41" name="use_for_d_predator"/>
-    <tableColumn id="40" name="use_for_rift_beast_fire"/>
-    <tableColumn id="46" name="use_for_rift_beast_ice"/>
-    <tableColumn id="45" name="use_for_rift_beast_wind"/>
-    <tableColumn id="44" name="use_for_rift_beast_light"/>
-    <tableColumn id="43" name="use_for_rift_beast_dark"/>
-    <tableColumn id="42" name="use_for_r5"/>
-    <tableColumn id="47" name="use_for_lab"/>
-    <tableColumn id="39" name="use_for_arena"/>
-    <tableColumn id="13" name="use_for_gwo"/>
-    <tableColumn id="15" name="use_for_gwd" dataDxfId="13"/>
-    <tableColumn id="12" name="use_for_rta" dataDxfId="12"/>
-    <tableColumn id="18" name="spd_tune_max" dataDxfId="11"/>
-    <tableColumn id="19" name="spd_tune_atk_bar" dataDxfId="10"/>
-    <tableColumn id="20" name="spd_tune_buffer" dataDxfId="9"/>
-    <tableColumn id="21" name="spd_tune_strip" dataDxfId="8"/>
-    <tableColumn id="22" name="spd_tune_debuff" dataDxfId="7"/>
-    <tableColumn id="23" name="spd_tune_dmg" dataDxfId="6"/>
-    <tableColumn id="8" name="cleanser" dataDxfId="5"/>
-    <tableColumn id="9" name="reviver" dataDxfId="4"/>
-    <tableColumn id="10" name="controller" dataDxfId="3"/>
-    <tableColumn id="7" name="runed_as_healer" dataDxfId="2"/>
-    <tableColumn id="6" name="runed_as_tank" dataDxfId="1"/>
-    <tableColumn id="5" name="runed_as_bruiser" dataDxfId="0"/>
-    <tableColumn id="4" name="player_unit_select_ignore"/>
+    <tableColumn id="2" name="name_ignore"/>
+    <tableColumn id="3" name="lvl_ignore"/>
+    <tableColumn id="4" name="use_for_gb12"/>
+    <tableColumn id="5" name="use_for_db12"/>
+    <tableColumn id="6" name="use_for_nb12"/>
+    <tableColumn id="7" name="use_for_sf10"/>
+    <tableColumn id="8" name="use_for_pc10"/>
+    <tableColumn id="9" name="use_for_toa"/>
+    <tableColumn id="10" name="use_for_dhole_griffon"/>
+    <tableColumn id="11" name="use_for_dhole_inugami"/>
+    <tableColumn id="12" name="use_for_dhole_warbear"/>
+    <tableColumn id="13" name="use_for_dhole_fairy"/>
+    <tableColumn id="14" name="use_for_dhole_pixie"/>
+    <tableColumn id="15" name="use_for_dhole_werewolf"/>
+    <tableColumn id="16" name="use_for_dhole_cat"/>
+    <tableColumn id="17" name="use_for_dhole_howl"/>
+    <tableColumn id="18" name="use_for_dhole_grim"/>
+    <tableColumn id="19" name="use_for_dhole_karzhan"/>
+    <tableColumn id="20" name="use_for_dhole_ellunia"/>
+    <tableColumn id="21" name="use_for_dhole_lumel"/>
+    <tableColumn id="22" name="use_for_dhole_khalderun"/>
+    <tableColumn id="23" name="use_for_d_predator"/>
+    <tableColumn id="24" name="use_for_rift_beast_fire"/>
+    <tableColumn id="25" name="use_for_rift_beast_ice"/>
+    <tableColumn id="26" name="use_for_rift_beast_wind"/>
+    <tableColumn id="27" name="use_for_rift_beast_light"/>
+    <tableColumn id="28" name="use_for_rift_beast_dark"/>
+    <tableColumn id="29" name="use_for_r5"/>
+    <tableColumn id="30" name="use_for_lab"/>
+    <tableColumn id="31" name="use_for_arena"/>
+    <tableColumn id="32" name="use_for_gwo"/>
+    <tableColumn id="33" name="use_for_gwd" dataDxfId="14"/>
+    <tableColumn id="34" name="use_for_rta" dataDxfId="13"/>
+    <tableColumn id="35" name="spd_tune_max" dataDxfId="12"/>
+    <tableColumn id="36" name="spd_tune_atk_bar" dataDxfId="11"/>
+    <tableColumn id="37" name="spd_tune_buffer" dataDxfId="10"/>
+    <tableColumn id="38" name="buffs" dataDxfId="9"/>
+    <tableColumn id="39" name="spd_tune_strip" dataDxfId="8"/>
+    <tableColumn id="40" name="spd_tune_debuff" dataDxfId="7"/>
+    <tableColumn id="41" name="debuffs" dataDxfId="6"/>
+    <tableColumn id="42" name="spd_tune_dmg" dataDxfId="5"/>
+    <tableColumn id="43" name="cleanser" dataDxfId="4"/>
+    <tableColumn id="44" name="reviver" dataDxfId="3"/>
+    <tableColumn id="46" name="runed_as_healer" dataDxfId="2"/>
+    <tableColumn id="47" name="runed_as_tank" dataDxfId="1"/>
+    <tableColumn id="48" name="runed_as_bruiser" dataDxfId="0"/>
+    <tableColumn id="49" name="player_unit_select_ignore"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -874,1522 +924,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU161"/>
+  <dimension ref="A1:AV1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="25.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="62.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="25.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="24.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="62.453125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:48" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AM1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AO1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AP1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AR1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AS1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AT1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AU1" s="8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>999999</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="AV1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C2">
-        <v>40</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="AB2">
-        <v>1</v>
-      </c>
-      <c r="AF2">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="5">
-        <v>1</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="AC3"/>
-      <c r="AF3"/>
-      <c r="AU3"/>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="I4"/>
-      <c r="AE4"/>
-      <c r="AU4"/>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="I5"/>
-      <c r="AE5"/>
-      <c r="AF5"/>
-      <c r="AR5"/>
-      <c r="AU5"/>
-    </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="Y6"/>
-      <c r="AE6"/>
-      <c r="AF6"/>
-      <c r="AU6"/>
-    </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="AF7"/>
-      <c r="AU7"/>
-    </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="AF8"/>
-      <c r="AU8"/>
-    </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="H9"/>
-      <c r="Z9"/>
-      <c r="AB9"/>
-      <c r="AC9"/>
-      <c r="AF9"/>
-      <c r="AU9"/>
-    </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="AF10"/>
-      <c r="AU10"/>
-    </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="AC11"/>
-      <c r="AU11"/>
-    </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="AU12"/>
-    </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="X13"/>
-      <c r="Y13"/>
-      <c r="Z13"/>
-      <c r="AA13"/>
-      <c r="AB13"/>
-      <c r="AF13"/>
-      <c r="AU13"/>
-    </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="AF14"/>
-      <c r="AU14"/>
-    </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="AD15"/>
-      <c r="AE15"/>
-      <c r="AF15"/>
-      <c r="AU15"/>
-    </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="I16"/>
-      <c r="AF16"/>
-      <c r="AU16"/>
-    </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="AF17"/>
-      <c r="AU17"/>
-    </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="Y18"/>
-      <c r="AF18"/>
-      <c r="AU18"/>
-    </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="Z19"/>
-      <c r="AC19"/>
-      <c r="AF19"/>
-      <c r="AU19"/>
-    </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="AF20"/>
-      <c r="AU20"/>
-    </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="AU21"/>
-    </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="I22"/>
-      <c r="AD22"/>
-      <c r="AF22"/>
-      <c r="AU22"/>
-    </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="H23"/>
-      <c r="AF23"/>
-      <c r="AU23"/>
-    </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="AF24"/>
-      <c r="AU24"/>
-    </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="AF25"/>
-      <c r="AU25"/>
-    </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="AC26"/>
-      <c r="AF26"/>
-      <c r="AU26"/>
-    </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="X27"/>
-      <c r="Y27"/>
-      <c r="Z27"/>
-      <c r="AA27"/>
-      <c r="AB27"/>
-      <c r="AC27"/>
-      <c r="AE27"/>
-      <c r="AF27"/>
-      <c r="AU27"/>
-    </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="O28"/>
-      <c r="X28"/>
-      <c r="AE28"/>
-      <c r="AF28"/>
-      <c r="AU28"/>
-    </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="AE29"/>
-      <c r="AF29"/>
-      <c r="AU29"/>
-    </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="AU30"/>
-    </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="E31"/>
-      <c r="I31"/>
-      <c r="J31"/>
-      <c r="K31"/>
-      <c r="O31"/>
-      <c r="P31"/>
-      <c r="AC31"/>
-      <c r="AE31"/>
-      <c r="AF31"/>
-      <c r="AU31"/>
-    </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="AE32"/>
-      <c r="AF32"/>
-      <c r="AU32"/>
-    </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="I33"/>
-      <c r="AD33"/>
-      <c r="AF33"/>
-      <c r="AU33"/>
-    </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="I34"/>
-      <c r="AU34"/>
-    </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="AE35"/>
-      <c r="AF35"/>
-      <c r="AU35"/>
-    </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="AU36"/>
-    </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="AU37"/>
-    </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="AF38"/>
-      <c r="AU38"/>
-    </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="AU39"/>
-    </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="Z40"/>
-      <c r="AA40"/>
-      <c r="AF40"/>
-      <c r="AU40"/>
-    </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="AC41"/>
-      <c r="AF41"/>
-      <c r="AU41"/>
-    </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A42"/>
-      <c r="B42"/>
-      <c r="C42"/>
-      <c r="E42"/>
-      <c r="F42"/>
-      <c r="H42"/>
-      <c r="I42"/>
-      <c r="Z42"/>
-      <c r="AA42"/>
-      <c r="AB42"/>
-      <c r="AF42"/>
-      <c r="AU42"/>
-    </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A43"/>
-      <c r="B43"/>
-      <c r="C43"/>
-      <c r="E43"/>
-      <c r="F43"/>
-      <c r="I43"/>
-      <c r="AF43"/>
-      <c r="AU43"/>
-    </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A44"/>
-      <c r="B44"/>
-      <c r="C44"/>
-      <c r="X44"/>
-      <c r="Y44"/>
-      <c r="AA44"/>
-      <c r="AF44"/>
-      <c r="AU44"/>
-    </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A45"/>
-      <c r="B45"/>
-      <c r="C45"/>
-      <c r="D45"/>
-      <c r="AU45"/>
-    </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A46"/>
-      <c r="B46"/>
-      <c r="C46"/>
-      <c r="AE46"/>
-      <c r="AF46"/>
-      <c r="AU46"/>
-    </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A47"/>
-      <c r="B47"/>
-      <c r="C47"/>
-      <c r="I47"/>
-      <c r="AD47"/>
-      <c r="AF47"/>
-      <c r="AU47"/>
-    </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A48"/>
-      <c r="B48"/>
-      <c r="C48"/>
-      <c r="F48"/>
-      <c r="AF48"/>
-      <c r="AU48"/>
-    </row>
-    <row r="49" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A49"/>
-      <c r="B49"/>
-      <c r="C49"/>
-      <c r="AE49"/>
-      <c r="AF49"/>
-      <c r="AU49"/>
-    </row>
-    <row r="50" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A50"/>
-      <c r="B50"/>
-      <c r="C50"/>
-      <c r="AU50"/>
-    </row>
-    <row r="51" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A51"/>
-      <c r="B51"/>
-      <c r="C51"/>
-      <c r="I51"/>
-      <c r="AF51"/>
-      <c r="AU51"/>
-    </row>
-    <row r="52" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A52"/>
-      <c r="B52"/>
-      <c r="C52"/>
-      <c r="X52"/>
-      <c r="Y52"/>
-      <c r="AA52"/>
-      <c r="AF52"/>
-      <c r="AU52"/>
-    </row>
-    <row r="53" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A53"/>
-      <c r="B53"/>
-      <c r="C53"/>
-      <c r="D53"/>
-      <c r="AU53"/>
-    </row>
-    <row r="54" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A54"/>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="AF54"/>
-      <c r="AU54"/>
-    </row>
-    <row r="55" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A55"/>
-      <c r="B55"/>
-      <c r="C55"/>
-      <c r="AE55"/>
-      <c r="AF55"/>
-      <c r="AU55"/>
-    </row>
-    <row r="56" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A56"/>
-      <c r="B56"/>
-      <c r="C56"/>
-      <c r="AF56"/>
-      <c r="AU56"/>
-    </row>
-    <row r="57" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A57"/>
-      <c r="B57"/>
-      <c r="C57"/>
-      <c r="E57"/>
-      <c r="H57"/>
-      <c r="I57"/>
-      <c r="J57"/>
-      <c r="K57"/>
-      <c r="P57"/>
-      <c r="AD57"/>
-      <c r="AF57"/>
-      <c r="AU57"/>
-    </row>
-    <row r="58" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A58"/>
-      <c r="B58"/>
-      <c r="C58"/>
-      <c r="I58"/>
-      <c r="AF58"/>
-      <c r="AU58"/>
-    </row>
-    <row r="59" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A59"/>
-      <c r="B59"/>
-      <c r="C59"/>
-      <c r="AF59"/>
-      <c r="AU59"/>
-    </row>
-    <row r="60" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A60"/>
-      <c r="B60"/>
-      <c r="C60"/>
-      <c r="F60"/>
-      <c r="AU60"/>
-    </row>
-    <row r="61" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A61"/>
-      <c r="B61"/>
-      <c r="C61"/>
-      <c r="X61"/>
-      <c r="AU61"/>
-    </row>
-    <row r="62" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A62"/>
-      <c r="B62"/>
-      <c r="C62"/>
-      <c r="AB62"/>
-      <c r="AC62"/>
-      <c r="AF62"/>
-      <c r="AU62"/>
-    </row>
-    <row r="63" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A63"/>
-      <c r="B63"/>
-      <c r="C63"/>
-      <c r="H63"/>
-      <c r="AU63"/>
-    </row>
-    <row r="64" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A64"/>
-      <c r="B64"/>
-      <c r="C64"/>
-      <c r="AU64"/>
-    </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A65"/>
-      <c r="B65"/>
-      <c r="C65"/>
-      <c r="AF65"/>
-      <c r="AU65"/>
-    </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A66"/>
-      <c r="B66"/>
-      <c r="C66"/>
-      <c r="AF66"/>
-      <c r="AU66"/>
-    </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A67"/>
-      <c r="B67"/>
-      <c r="C67"/>
-      <c r="AF67"/>
-      <c r="AU67"/>
-    </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A68"/>
-      <c r="B68"/>
-      <c r="C68"/>
-      <c r="AU68"/>
-    </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A69"/>
-      <c r="B69"/>
-      <c r="C69"/>
-      <c r="AF69"/>
-      <c r="AU69"/>
-    </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A70"/>
-      <c r="B70"/>
-      <c r="C70"/>
-      <c r="AF70"/>
-      <c r="AU70"/>
-    </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A71"/>
-      <c r="B71"/>
-      <c r="C71"/>
-      <c r="AF71"/>
-      <c r="AU71"/>
-    </row>
-    <row r="72" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A72"/>
-      <c r="B72"/>
-      <c r="C72"/>
-      <c r="AF72"/>
-      <c r="AU72"/>
-    </row>
-    <row r="73" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A73"/>
-      <c r="B73"/>
-      <c r="C73"/>
-      <c r="AU73"/>
-    </row>
-    <row r="74" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A74"/>
-      <c r="B74"/>
-      <c r="C74"/>
-      <c r="AF74"/>
-      <c r="AG74"/>
-      <c r="AS74"/>
-      <c r="AU74"/>
-    </row>
-    <row r="75" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A75"/>
-      <c r="B75"/>
-      <c r="C75"/>
-      <c r="AF75"/>
-      <c r="AM75"/>
-      <c r="AU75"/>
-    </row>
-    <row r="76" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A76"/>
-      <c r="B76"/>
-      <c r="C76"/>
-      <c r="AF76"/>
-      <c r="AR76"/>
-      <c r="AU76"/>
-    </row>
-    <row r="77" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A77"/>
-      <c r="B77"/>
-      <c r="C77"/>
-      <c r="AF77"/>
-      <c r="AK77"/>
-      <c r="AL77"/>
-      <c r="AU77"/>
-    </row>
-    <row r="78" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A78"/>
-      <c r="B78"/>
-      <c r="C78"/>
-      <c r="AF78"/>
-      <c r="AI78"/>
-      <c r="AR78"/>
-      <c r="AU78"/>
-    </row>
-    <row r="79" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A79"/>
-      <c r="B79"/>
-      <c r="C79"/>
-      <c r="AF79"/>
-      <c r="AG79"/>
-      <c r="AL79"/>
-      <c r="AU79"/>
-    </row>
-    <row r="80" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A80"/>
-      <c r="B80"/>
-      <c r="C80"/>
-      <c r="AF80"/>
-      <c r="AM80"/>
-      <c r="AU80"/>
-    </row>
-    <row r="81" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A81"/>
-      <c r="B81"/>
-      <c r="C81"/>
-      <c r="AF81"/>
-      <c r="AR81"/>
-      <c r="AU81"/>
-    </row>
-    <row r="82" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A82"/>
-      <c r="B82"/>
-      <c r="C82"/>
-      <c r="AF82"/>
-      <c r="AG82"/>
-      <c r="AJ82"/>
-      <c r="AK82"/>
-      <c r="AU82"/>
-    </row>
-    <row r="83" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A83"/>
-      <c r="B83"/>
-      <c r="C83"/>
-      <c r="AF83"/>
-      <c r="AU83"/>
-    </row>
-    <row r="84" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A84"/>
-      <c r="B84"/>
-      <c r="C84"/>
-      <c r="AF84"/>
-      <c r="AN84"/>
-      <c r="AU84"/>
-    </row>
-    <row r="85" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A85"/>
-      <c r="B85"/>
-      <c r="C85"/>
-      <c r="AF85"/>
-      <c r="AG85"/>
-      <c r="AK85"/>
-      <c r="AL85"/>
-      <c r="AR85"/>
-      <c r="AU85"/>
-    </row>
-    <row r="86" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A86"/>
-      <c r="B86"/>
-      <c r="C86"/>
-      <c r="AN86"/>
-      <c r="AU86"/>
-    </row>
-    <row r="87" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A87"/>
-      <c r="B87"/>
-      <c r="C87"/>
-      <c r="AU87"/>
-    </row>
-    <row r="88" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A88"/>
-      <c r="B88"/>
-      <c r="C88"/>
-      <c r="AF88"/>
-      <c r="AR88"/>
-      <c r="AU88"/>
-    </row>
-    <row r="89" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A89"/>
-      <c r="B89"/>
-      <c r="C89"/>
-      <c r="AF89"/>
-      <c r="AM89"/>
-      <c r="AU89"/>
-    </row>
-    <row r="90" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A90"/>
-      <c r="B90"/>
-      <c r="C90"/>
-      <c r="AF90"/>
-      <c r="AG90"/>
-      <c r="AH90"/>
-      <c r="AQ90"/>
-      <c r="AU90"/>
-    </row>
-    <row r="91" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A91"/>
-      <c r="B91"/>
-      <c r="C91"/>
-      <c r="AF91"/>
-      <c r="AT91"/>
-      <c r="AU91"/>
-    </row>
-    <row r="92" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A92"/>
-      <c r="B92"/>
-      <c r="C92"/>
-      <c r="AF92"/>
-      <c r="AS92"/>
-      <c r="AU92"/>
-    </row>
-    <row r="93" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A93"/>
-      <c r="B93"/>
-      <c r="C93"/>
-      <c r="AF93"/>
-      <c r="AL93"/>
-      <c r="AM93"/>
-      <c r="AU93"/>
-    </row>
-    <row r="94" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A94"/>
-      <c r="B94"/>
-      <c r="C94"/>
-      <c r="AF94"/>
-      <c r="AG94"/>
-      <c r="AS94"/>
-      <c r="AU94"/>
-    </row>
-    <row r="95" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A95"/>
-      <c r="B95"/>
-      <c r="C95"/>
-      <c r="AF95"/>
-      <c r="AK95"/>
-      <c r="AR95"/>
-      <c r="AU95"/>
-    </row>
-    <row r="96" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A96"/>
-      <c r="B96"/>
-      <c r="C96"/>
-      <c r="AF96"/>
-      <c r="AN96"/>
-      <c r="AU96"/>
-    </row>
-    <row r="97" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A97"/>
-      <c r="B97"/>
-      <c r="C97"/>
-      <c r="AF97"/>
-      <c r="AG97"/>
-      <c r="AR97"/>
-      <c r="AU97"/>
-    </row>
-    <row r="98" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A98"/>
-      <c r="B98"/>
-      <c r="C98"/>
-      <c r="AF98"/>
-      <c r="AU98"/>
-    </row>
-    <row r="99" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A99"/>
-      <c r="B99"/>
-      <c r="C99"/>
-      <c r="AF99"/>
-      <c r="AG99"/>
-      <c r="AO99"/>
-      <c r="AU99"/>
-    </row>
-    <row r="100" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A100"/>
-      <c r="B100"/>
-      <c r="C100"/>
-      <c r="AM100"/>
-      <c r="AU100"/>
-    </row>
-    <row r="101" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A101"/>
-      <c r="B101"/>
-      <c r="C101"/>
-      <c r="AU101"/>
-    </row>
-    <row r="102" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A102"/>
-      <c r="B102"/>
-      <c r="C102"/>
-      <c r="AU102"/>
-    </row>
-    <row r="103" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A103"/>
-      <c r="B103"/>
-      <c r="C103"/>
-      <c r="AF103"/>
-      <c r="AG103"/>
-      <c r="AM103"/>
-      <c r="AU103"/>
-    </row>
-    <row r="104" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A104"/>
-      <c r="B104"/>
-      <c r="C104"/>
-      <c r="AF104"/>
-      <c r="AQ104"/>
-      <c r="AU104"/>
-    </row>
-    <row r="105" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A105"/>
-      <c r="B105"/>
-      <c r="C105"/>
-      <c r="AF105"/>
-      <c r="AK105"/>
-      <c r="AO105"/>
-      <c r="AU105"/>
-    </row>
-    <row r="106" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A106"/>
-      <c r="B106"/>
-      <c r="C106"/>
-      <c r="AU106"/>
-    </row>
-    <row r="107" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A107"/>
-      <c r="B107"/>
-      <c r="C107"/>
-      <c r="AF107"/>
-      <c r="AU107"/>
-    </row>
-    <row r="108" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A108"/>
-      <c r="B108"/>
-      <c r="C108"/>
-      <c r="AF108"/>
-      <c r="AN108"/>
-      <c r="AU108"/>
-    </row>
-    <row r="109" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A109"/>
-      <c r="B109"/>
-      <c r="C109"/>
-      <c r="AF109"/>
-      <c r="AH109"/>
-      <c r="AL109"/>
-      <c r="AR109"/>
-      <c r="AU109"/>
-    </row>
-    <row r="110" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A110"/>
-      <c r="B110"/>
-      <c r="C110"/>
-      <c r="AE110"/>
-      <c r="AF110"/>
-      <c r="AJ110"/>
-      <c r="AU110"/>
-    </row>
-    <row r="111" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A111"/>
-      <c r="B111"/>
-      <c r="C111"/>
-      <c r="AF111"/>
-      <c r="AN111"/>
-      <c r="AU111"/>
-    </row>
-    <row r="112" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A112"/>
-      <c r="B112"/>
-      <c r="C112"/>
-      <c r="AF112"/>
-      <c r="AU112"/>
-    </row>
-    <row r="113" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A113"/>
-      <c r="B113"/>
-      <c r="C113"/>
-      <c r="AF113"/>
-      <c r="AU113"/>
-    </row>
-    <row r="114" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A114"/>
-      <c r="B114"/>
-      <c r="C114"/>
-      <c r="AF114"/>
-      <c r="AG114"/>
-      <c r="AU114"/>
-    </row>
-    <row r="115" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A115"/>
-      <c r="B115"/>
-      <c r="C115"/>
-      <c r="AU115"/>
-    </row>
-    <row r="116" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A116"/>
-      <c r="B116"/>
-      <c r="C116"/>
-      <c r="AF116"/>
-      <c r="AL116"/>
-      <c r="AU116"/>
-    </row>
-    <row r="117" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A117"/>
-      <c r="B117"/>
-      <c r="C117"/>
-      <c r="AU117"/>
-    </row>
-    <row r="118" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A118"/>
-      <c r="B118"/>
-      <c r="C118"/>
-      <c r="AF118"/>
-      <c r="AN118"/>
-      <c r="AU118"/>
-    </row>
-    <row r="119" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A119"/>
-      <c r="B119"/>
-      <c r="C119"/>
-      <c r="AF119"/>
-      <c r="AU119"/>
-    </row>
-    <row r="120" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A120"/>
-      <c r="B120"/>
-      <c r="C120"/>
-      <c r="AF120"/>
-      <c r="AQ120"/>
-      <c r="AU120"/>
-    </row>
-    <row r="121" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A121"/>
-      <c r="B121"/>
-      <c r="C121"/>
-      <c r="AF121"/>
-      <c r="AM121"/>
-      <c r="AU121"/>
-    </row>
-    <row r="122" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A122"/>
-      <c r="B122"/>
-      <c r="C122"/>
-      <c r="AU122"/>
-    </row>
-    <row r="123" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A123"/>
-      <c r="B123"/>
-      <c r="C123"/>
-      <c r="AF123"/>
-      <c r="AN123"/>
-      <c r="AU123"/>
-    </row>
-    <row r="124" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A124"/>
-      <c r="B124"/>
-      <c r="C124"/>
-      <c r="AF124"/>
-      <c r="AP124"/>
-      <c r="AR124"/>
-      <c r="AU124"/>
-    </row>
-    <row r="125" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A125"/>
-      <c r="B125"/>
-      <c r="C125"/>
-      <c r="AF125"/>
-      <c r="AN125"/>
-      <c r="AU125"/>
-    </row>
-    <row r="126" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A126"/>
-      <c r="B126"/>
-      <c r="C126"/>
-      <c r="AF126"/>
-      <c r="AO126"/>
-      <c r="AR126"/>
-      <c r="AU126"/>
-    </row>
-    <row r="127" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A127"/>
-      <c r="B127"/>
-      <c r="C127"/>
-      <c r="AF127"/>
-      <c r="AH127"/>
-      <c r="AU127"/>
-    </row>
-    <row r="128" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A128"/>
-      <c r="B128"/>
-      <c r="C128"/>
-      <c r="AU128"/>
-    </row>
-    <row r="129" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A129"/>
-      <c r="B129"/>
-      <c r="C129"/>
-      <c r="AF129"/>
-      <c r="AN129"/>
-      <c r="AU129"/>
-    </row>
-    <row r="130" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A130"/>
-      <c r="B130"/>
-      <c r="C130"/>
-      <c r="AF130"/>
-      <c r="AU130"/>
-    </row>
-    <row r="131" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A131"/>
-      <c r="B131"/>
-      <c r="C131"/>
-      <c r="AF131"/>
-      <c r="AG131"/>
-      <c r="AJ131"/>
-      <c r="AU131"/>
-    </row>
-    <row r="132" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A132"/>
-      <c r="B132"/>
-      <c r="C132"/>
-      <c r="AF132"/>
-      <c r="AH132"/>
-      <c r="AL132"/>
-      <c r="AQ132"/>
-      <c r="AU132"/>
-    </row>
-    <row r="133" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A133"/>
-      <c r="B133"/>
-      <c r="C133"/>
-      <c r="AF133"/>
-      <c r="AG133"/>
-      <c r="AJ133"/>
-      <c r="AK133"/>
-      <c r="AO133"/>
-      <c r="AU133"/>
-    </row>
-    <row r="134" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A134"/>
-      <c r="B134"/>
-      <c r="C134"/>
-      <c r="AF134"/>
-      <c r="AO134"/>
-      <c r="AU134"/>
-    </row>
-    <row r="135" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A135"/>
-      <c r="B135"/>
-      <c r="C135"/>
-      <c r="AF135"/>
-      <c r="AG135"/>
-      <c r="AR135"/>
-      <c r="AS135"/>
-      <c r="AU135"/>
-    </row>
-    <row r="136" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A136"/>
-      <c r="B136"/>
-      <c r="C136"/>
-      <c r="AF136"/>
-      <c r="AL136"/>
-      <c r="AU136"/>
-    </row>
-    <row r="137" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A137"/>
-      <c r="B137"/>
-      <c r="C137"/>
-      <c r="AF137"/>
-      <c r="AK137"/>
-      <c r="AU137"/>
-    </row>
-    <row r="138" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A138"/>
-      <c r="B138"/>
-      <c r="C138"/>
-      <c r="AU138"/>
-    </row>
-    <row r="139" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A139"/>
-      <c r="B139"/>
-      <c r="C139"/>
-      <c r="AU139"/>
-    </row>
-    <row r="140" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A140"/>
-      <c r="B140"/>
-      <c r="C140"/>
-      <c r="AF140"/>
-      <c r="AG140"/>
-      <c r="AN140"/>
-      <c r="AU140"/>
-    </row>
-    <row r="141" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A141"/>
-      <c r="B141"/>
-      <c r="C141"/>
-      <c r="AF141"/>
-      <c r="AG141"/>
-      <c r="AU141"/>
-    </row>
-    <row r="142" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A142"/>
-      <c r="B142"/>
-      <c r="C142"/>
-      <c r="AU142"/>
-    </row>
-    <row r="143" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A143"/>
-      <c r="B143"/>
-      <c r="C143"/>
-      <c r="AU143"/>
-    </row>
-    <row r="144" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A144"/>
-      <c r="B144"/>
-      <c r="C144"/>
-      <c r="AU144"/>
-    </row>
-    <row r="145" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A145"/>
-      <c r="B145"/>
-      <c r="C145"/>
-      <c r="AF145"/>
-      <c r="AM145"/>
-      <c r="AT145"/>
-      <c r="AU145"/>
-    </row>
-    <row r="146" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A146"/>
-      <c r="B146"/>
-      <c r="C146"/>
-      <c r="AU146"/>
-    </row>
-    <row r="147" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A147"/>
-      <c r="B147"/>
-      <c r="C147"/>
-      <c r="AF147"/>
-      <c r="AK147"/>
-      <c r="AS147"/>
-      <c r="AU147"/>
-    </row>
-    <row r="148" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A148"/>
-      <c r="B148"/>
-      <c r="C148"/>
-      <c r="AF148"/>
-      <c r="AU148"/>
-    </row>
-    <row r="149" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A149"/>
-      <c r="B149"/>
-      <c r="C149"/>
-      <c r="AF149"/>
-      <c r="AN149"/>
-      <c r="AU149"/>
-    </row>
-    <row r="150" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A150"/>
-      <c r="B150"/>
-      <c r="C150"/>
-      <c r="AU150"/>
-    </row>
-    <row r="151" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A151"/>
-      <c r="B151"/>
-      <c r="C151"/>
-      <c r="AF151"/>
-      <c r="AG151"/>
-      <c r="AK151"/>
-      <c r="AP151"/>
-      <c r="AR151"/>
-      <c r="AU151"/>
-    </row>
-    <row r="152" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A152"/>
-      <c r="B152"/>
-      <c r="C152"/>
-      <c r="AF152"/>
-      <c r="AG152"/>
-      <c r="AO152"/>
-      <c r="AR152"/>
-      <c r="AU152"/>
-    </row>
-    <row r="153" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A153"/>
-      <c r="B153"/>
-      <c r="C153"/>
-      <c r="AF153"/>
-      <c r="AG153"/>
-      <c r="AM153"/>
-      <c r="AU153"/>
-    </row>
-    <row r="154" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A154"/>
-      <c r="B154"/>
-      <c r="C154"/>
-      <c r="AF154"/>
-      <c r="AR154"/>
-      <c r="AU154"/>
-    </row>
-    <row r="155" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A155"/>
-      <c r="B155"/>
-      <c r="C155"/>
-      <c r="AF155"/>
-      <c r="AN155"/>
-      <c r="AU155"/>
-    </row>
-    <row r="156" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A156"/>
-      <c r="B156"/>
-      <c r="C156"/>
-      <c r="AF156"/>
-      <c r="AG156"/>
-      <c r="AH156"/>
-      <c r="AO156"/>
-      <c r="AR156"/>
-      <c r="AU156"/>
-    </row>
-    <row r="157" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A157"/>
-      <c r="B157"/>
-      <c r="C157"/>
-      <c r="AF157"/>
-      <c r="AG157"/>
-      <c r="AN157"/>
-      <c r="AQ157"/>
-      <c r="AU157"/>
-    </row>
-    <row r="158" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A158"/>
-      <c r="B158"/>
-      <c r="C158"/>
-      <c r="AF158"/>
-      <c r="AJ158"/>
-      <c r="AU158"/>
-    </row>
-    <row r="159" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A159"/>
-      <c r="B159"/>
-      <c r="C159"/>
-      <c r="AF159"/>
-      <c r="AT159"/>
-      <c r="AU159"/>
-    </row>
-    <row r="160" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A160"/>
-      <c r="B160"/>
-      <c r="C160"/>
-      <c r="AU160"/>
-    </row>
-    <row r="161" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A161"/>
-      <c r="B161"/>
-      <c r="C161"/>
-      <c r="AF161"/>
-      <c r="AN161"/>
-      <c r="AU161"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2409,18 +1147,18 @@
       <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="14" width="8.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="8.7265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
@@ -2440,7 +1178,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2461,7 +1199,7 @@
         <v>No Team - Low Priority | 1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2482,7 +1220,7 @@
         <v>No Team - Medium Priority | 2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2503,7 +1241,7 @@
         <v>No Team - High Priority | 3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2524,7 +1262,7 @@
         <v>Farmer / Rep | 4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2545,7 +1283,7 @@
         <v>Giant's Keep | 5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2566,7 +1304,7 @@
         <v>Dragon's Lair | 6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2587,7 +1325,7 @@
         <v>Necropolis | 7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2608,7 +1346,7 @@
         <v>Steal Fortress | 8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2629,7 +1367,7 @@
         <v>Punisher's Crypt | 9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2650,7 +1388,7 @@
         <v>Hall of Magic | 10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2671,7 +1409,7 @@
         <v>Hall of Light | 11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2692,7 +1430,7 @@
         <v>Hall of Dark | 12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2713,7 +1451,7 @@
         <v>Hall of Fire | 13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2734,7 +1472,7 @@
         <v>Hall of Water | 14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2755,7 +1493,7 @@
         <v>Hall of Wind | 15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2776,7 +1514,7 @@
         <v>Hall of Heroes | 16</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2797,7 +1535,7 @@
         <v>Trial of Ascension (Normal) | 17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2818,7 +1556,7 @@
         <v>Trial of Ascension (Hard) | 18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2839,7 +1577,7 @@
         <v>Trial of Ascension (Hell) | 19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2860,7 +1598,7 @@
         <v>Karzhan Remains - Griffon Lvl 4 (Dark) | 20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2881,7 +1619,7 @@
         <v>Karzhan Remains - Griffon Lvl 5 (Wind) | 21</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2902,7 +1640,7 @@
         <v>Karzhan Remains - Inugami Lvl 4 (Light) | 22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2923,7 +1661,7 @@
         <v>Karzhan Remains - Inugami Lvl 5 (Dark) | 23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2944,7 +1682,7 @@
         <v>Karzhan Remains - Warbear Lvl 4 (Dark) | 24</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2965,7 +1703,7 @@
         <v>Karzhan Remains - Warbear Lvl 5 (Fire) | 25</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2986,7 +1724,7 @@
         <v>Ellunia Remains -  Fairy Lvl 4 (Wind) | 26</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3007,7 +1745,7 @@
         <v>Ellunia Remains -  Fairy Lvl 5 (Light) | 27</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3028,7 +1766,7 @@
         <v>Ellunia Remains -  Pixie Lvl 4 (Wind) | 28</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3049,7 +1787,7 @@
         <v>Ellunia Remains -  Pixie Lvl 5 (Water) | 29</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3070,7 +1808,7 @@
         <v>Lumel Remains - Werewolf Lvl 4 (Light) | 30</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -3091,7 +1829,7 @@
         <v>Lumel Remains - Werewolf Lvl 5 (Fire) | 31</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -3112,7 +1850,7 @@
         <v>Lumel Remains - Martial Cat Lvl 4 (Dark) | 32</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -3133,7 +1871,7 @@
         <v>Lumel Remains - Martial Cat Lvl 5 (Wind) | 33</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3154,7 +1892,7 @@
         <v>Khalderun Remains - Howl Lvl 4 (Fire) | 34</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -3175,7 +1913,7 @@
         <v>Khalderun Remains - Howl Lvl 5 (Water) | 35</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -3196,7 +1934,7 @@
         <v>Khalderun Remains - Grim Reaper Lvl 4 (Water) | 36</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3217,7 +1955,7 @@
         <v>Khalderun Remains - Grim Reaper Lvl 5 (Dark) | 37</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3238,7 +1976,7 @@
         <v>Karzhan - Forest of Roaring Beasts | 38</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3259,7 +1997,7 @@
         <v>Ellunia - Sanctuary of Dreaming Fairies | 39</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3280,7 +2018,7 @@
         <v>Lumel - Cliff of Beast Men | 40</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3301,7 +2039,7 @@
         <v>Khalderun - Ruin of Silent Death | 41</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3322,7 +2060,7 @@
         <v>Dimension Hole Predator (Fire) | 42</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3343,7 +2081,7 @@
         <v>Dimension Hole Predator (Water) | 43</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3364,7 +2102,7 @@
         <v>Dimension Hole Predator (Wind) | 44</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3385,7 +2123,7 @@
         <v>Dimension Hole Predator (Light) | 45</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3406,7 +2144,7 @@
         <v>Dimension Hole Predator (Dark) | 46</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3427,7 +2165,7 @@
         <v>Rift of Worlds - Fire Beast | 47</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3448,7 +2186,7 @@
         <v>Rift of Worlds - Ice Beast | 48</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3469,7 +2207,7 @@
         <v>Rift of Worlds - Wind Beast | 49</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3490,7 +2228,7 @@
         <v>Rift of Worlds - Light Beast | 50</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3511,7 +2249,7 @@
         <v>Rift of Worlds - Dark Beast | 51</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3532,7 +2270,7 @@
         <v>Rift Raid | 52</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3553,7 +2291,7 @@
         <v>Tartarus Labyrinth - Normal | 53</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3574,7 +2312,7 @@
         <v>Tartarus Labyrinth - Rescue | 54</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3595,7 +2333,7 @@
         <v>Tartarus Labyrinth - Explode | 55</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3616,7 +2354,7 @@
         <v>Tartarus Labyrinth - Cool Time | 56</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3637,7 +2375,7 @@
         <v>Tartarus Labyrinth - Speed Limit | 57</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3658,7 +2396,7 @@
         <v>Tartarus Labyrinth - Time Limit | 58</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3679,7 +2417,7 @@
         <v>Tartarus Labyrinth - Guilles | 59</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3700,7 +2438,7 @@
         <v>Tartarus Labyrinth - Kotos | 60</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -3721,7 +2459,7 @@
         <v>Tartarus Labyrinth - Leos | 61</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3742,7 +2480,7 @@
         <v>Tartarus Labyrinth - Tartarus | 62</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3763,7 +2501,7 @@
         <v>Guild War Offense | 63</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3784,7 +2522,7 @@
         <v>Guild War Defense | 64</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -3805,7 +2543,7 @@
         <v>Siege Battle Offense | 65</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3826,7 +2564,7 @@
         <v>Siege Battle Defense | 66</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -3847,7 +2585,7 @@
         <v>Arena Offense | 67</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -3868,7 +2606,7 @@
         <v>Arena Defense | 68</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>69</v>
       </c>

</xml_diff>